<commit_message>
modified code, delete waste code
</commit_message>
<xml_diff>
--- a/data/sinhvien_chieu_nhom11.xlsx
+++ b/data/sinhvien_chieu_nhom11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackg\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0713140-FC0C-46C0-9E30-D4AC29023F09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B358786F-63ED-4171-8F74-9D81A1EF1E9B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{86C20704-E102-467C-9C92-11DDE1E4B682}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{86C20704-E102-467C-9C92-11DDE1E4B682}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1137,24 +1137,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C4287D-1542-44A4-B813-6FA3AC886052}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="24.44140625" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>226</v>
       </c>
       <c r="H3" s="2">
-        <v>373554489</v>
+        <v>373554789</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>21</v>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1552,7 +1552,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1783,7 +1783,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1882,7 +1882,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1948,7 +1948,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2212,7 +2212,7 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2245,7 +2245,7 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2278,7 +2278,7 @@
       </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2443,7 +2443,7 @@
       </c>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2773,7 +2773,7 @@
       </c>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2839,7 +2839,7 @@
       </c>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2905,7 +2905,7 @@
       </c>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2938,7 +2938,7 @@
       </c>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3004,7 +3004,7 @@
       </c>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>

</xml_diff>